<commit_message>
automation of validation and analysis
</commit_message>
<xml_diff>
--- a/Sample_Task_name/tasks.xlsx
+++ b/Sample_Task_name/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Week</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Sample Images/download_figma_and_install.PNG</t>
+  </si>
+  <si>
+    <t>sample task</t>
+  </si>
+  <si>
+    <t>sample task1</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -512,6 +518,28 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>